<commit_message>
Add Individual Student Generate/Send Admit Card functionality
</commit_message>
<xml_diff>
--- a/HUTOPS/UploadedFiles/AdmitCardBatch/20231003145812.xlsx
+++ b/HUTOPS/UploadedFiles/AdmitCardBatch/20231003145812.xlsx
@@ -14,8 +14,9 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Result" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>HUTOPSIds</t>
   </si>
@@ -67,13 +68,20 @@
   </si>
   <si>
     <t>HUTOPS23-00012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Record not found </t>
+  </si>
+  <si>
+    <t>Result Updated Successfully</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -426,65 +434,167 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="1" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" s="0" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3">
+      <c r="A3" s="0" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4">
+      <c r="A4" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5">
+      <c r="A5" s="0" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6">
+      <c r="A6" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7">
+      <c r="A7" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8">
+      <c r="A8" s="0" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9">
+      <c r="A9" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10">
+      <c r="A10" s="0" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11">
+      <c r="A11" s="0" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>